<commit_message>
Added the invoice header
Added the invoice header and table
</commit_message>
<xml_diff>
--- a/app5-pdf-invoice-generator/invoices/10001-2023.1.18.xlsx
+++ b/app5-pdf-invoice-generator/invoices/10001-2023.1.18.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nttlimited-my.sharepoint.com/personal/rieda_hoosain_mweb_com/Documents/Software Dev/My Portfolio/app5-pdf-invoice-generator/invoices/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_E74022ED2B5D1D142EC46EDD4B4427FC95C7990E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{78A0C996-7BB1-4579-B3EC-F723AF222172}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>product_id</t>
   </si>
@@ -43,28 +52,15 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <sz val="15"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="1"/>
+      <b/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
@@ -205,45 +201,45 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="12">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -254,26 +250,89 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffbdc0bf"/>
-      <rgbColor rgb="ffa5a5a5"/>
-      <rgbColor rgb="ff3f3f3f"/>
-      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFBDC0BF"/>
+      <rgbColor rgb="FFA5A5A5"/>
+      <rgbColor rgb="FF3F3F3F"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Blank">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Blank">
   <a:themeElements>
     <a:clrScheme name="Blank">
       <a:dk1>
@@ -475,7 +534,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -494,7 +553,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -524,7 +583,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -550,7 +609,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -576,7 +635,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -602,7 +661,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -628,7 +687,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -654,7 +713,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -680,7 +739,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -706,7 +765,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -732,7 +791,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -745,9 +804,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -764,7 +829,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -783,7 +848,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -809,7 +874,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -835,7 +900,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -861,7 +926,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -887,7 +952,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -913,7 +978,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -939,7 +1004,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -965,7 +1030,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -991,7 +1056,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1017,7 +1082,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1030,9 +1095,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1046,7 +1117,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1065,7 +1136,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1095,7 +1166,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1121,7 +1192,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1147,7 +1218,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1173,7 +1244,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1199,7 +1270,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1225,7 +1296,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1251,7 +1322,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1277,7 +1348,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1303,7 +1374,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1316,54 +1387,63 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="13.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="13.9" customHeight="1"/>
   <cols>
-    <col min="1" max="6" width="16.3516" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="16.3516" style="1" customWidth="1"/>
+    <col min="1" max="7" width="16.28515625" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="16.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.7" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:6" ht="14.65" customHeight="1">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="2">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="2">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="2">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="2">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="3"/>
     </row>
-    <row r="2" ht="14.7" customHeight="1">
-      <c r="A2" t="s" s="4">
+    <row r="2" spans="1:6" ht="14.65" customHeight="1">
+      <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s" s="5">
+      <c r="B2" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="6">
@@ -1377,11 +1457,11 @@
       </c>
       <c r="F2" s="7"/>
     </row>
-    <row r="3" ht="26.7" customHeight="1">
-      <c r="A3" t="s" s="8">
+    <row r="3" spans="1:6" ht="26.65" customHeight="1">
+      <c r="A3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s" s="9">
+      <c r="B3" s="9" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="10">
@@ -1395,7 +1475,7 @@
       </c>
       <c r="F3" s="11"/>
     </row>
-    <row r="4" ht="14.35" customHeight="1">
+    <row r="4" spans="1:6" ht="14.45" customHeight="1">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
@@ -1403,7 +1483,7 @@
       <c r="E4" s="11"/>
       <c r="F4" s="11"/>
     </row>
-    <row r="5" ht="14.05" customHeight="1">
+    <row r="5" spans="1:6" ht="14.1" customHeight="1">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
@@ -1411,7 +1491,7 @@
       <c r="E5" s="11"/>
       <c r="F5" s="11"/>
     </row>
-    <row r="6" ht="14.05" customHeight="1">
+    <row r="6" spans="1:6" ht="14.1" customHeight="1">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
@@ -1419,7 +1499,7 @@
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
     </row>
-    <row r="7" ht="14.05" customHeight="1">
+    <row r="7" spans="1:6" ht="14.1" customHeight="1">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
@@ -1427,7 +1507,7 @@
       <c r="E7" s="11"/>
       <c r="F7" s="11"/>
     </row>
-    <row r="8" ht="14.05" customHeight="1">
+    <row r="8" spans="1:6" ht="14.1" customHeight="1">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
@@ -1435,7 +1515,7 @@
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
     </row>
-    <row r="9" ht="14.05" customHeight="1">
+    <row r="9" spans="1:6" ht="14.1" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
@@ -1443,7 +1523,7 @@
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
     </row>
-    <row r="10" ht="14.05" customHeight="1">
+    <row r="10" spans="1:6" ht="14.1" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -1453,9 +1533,9 @@
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P_x000D_&amp;1#&amp;"Arial"&amp;8&amp;K2E404D Sensitivity Label: General</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>